<commit_message>
dodělano vzorce pro převod na mbar
</commit_message>
<xml_diff>
--- a/mereni_MD/1.sval2.xlsx
+++ b/mereni_MD/1.sval2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarekDarsaU\Documents\Škola\5.Semester\Projekt-5\mereni_MD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MarekU\Programing\Projekt-5\mereni_MD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985F922C-535F-4102-82A0-281E2F7BA2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60B28B-093E-4C63-849E-59CA96DCF386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -849,7 +849,552 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hodnota fyzického senzoru</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10082808398950131"/>
+                  <c:y val="1.3135024788568095E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>615.73895263671795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>628.27087402343705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>647.91143798828102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>669.56915283203102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>687.469482421875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>716.30560302734295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>734.56219482421795</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>758.909423828125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>778.25231933593705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>807.80169677734295</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>831.05999755859295</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>851.46490478515602</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>874.50842285156205</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>894.92321777343705</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>918.85888671875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>943.45025634765602</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>962.58264160156205</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>986.54455566406205</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1007.42810058593</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1029.51062011718</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1069.84338378906</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1086.5615234375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1105.24401855468</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1133.93395996093</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1150.59423828125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1181.17822265625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1201.73913574218</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet!$C$2:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C031-4E8B-87BE-F72896D88CEC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1074929935"/>
+        <c:axId val="1980018159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1074929935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1980018159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1980018159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1074929935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1405,6 +1950,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1438,6 +2499,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EEC0B4D-3CE2-9D5F-C503-BA5BF871047A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1734,12 +2831,12 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +2850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1767,7 +2864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -1781,7 +2878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -1795,7 +2892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -1809,7 +2906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -1823,7 +2920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60</v>
       </c>
@@ -1837,7 +2934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70</v>
       </c>
@@ -1851,7 +2948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80</v>
       </c>
@@ -1865,7 +2962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90</v>
       </c>
@@ -1879,7 +2976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100</v>
       </c>
@@ -1893,7 +2990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
@@ -1907,7 +3004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -1921,7 +3018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>130</v>
       </c>
@@ -1935,7 +3032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>140</v>
       </c>
@@ -1949,7 +3046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>150</v>
       </c>
@@ -1963,7 +3060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>160</v>
       </c>
@@ -1977,7 +3074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>170</v>
       </c>
@@ -1991,7 +3088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>180</v>
       </c>
@@ -2005,7 +3102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>190</v>
       </c>
@@ -2019,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>200</v>
       </c>
@@ -2033,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>210</v>
       </c>
@@ -2047,7 +3144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>220</v>
       </c>
@@ -2061,7 +3158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>230</v>
       </c>
@@ -2075,7 +3172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>240</v>
       </c>
@@ -2089,7 +3186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>250</v>
       </c>
@@ -2103,7 +3200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>260</v>
       </c>
@@ -2117,7 +3214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>270</v>
       </c>

</xml_diff>